<commit_message>
Atualiza Planilha de Definição de Arquitetura
</commit_message>
<xml_diff>
--- a/Documentos/Arquitetura/Guia Definicao da Arquitetura V4.xlsx
+++ b/Documentos/Arquitetura/Guia Definicao da Arquitetura V4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isabella.silva\Desktop\Bandtec\3 semestre\miaudote\Documentos\Arquitetura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9744ED7B-848A-4291-8985-036D9C57BCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9FC819-8FE3-47AB-A335-1D2804C5927B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>MECANISMO DE IMPLEMENTAÇÃO</t>
   </si>
@@ -201,12 +201,6 @@
     <t>Wi-Fi, ETHERNET, 3G, 4G</t>
   </si>
   <si>
-    <t>Azure</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>Trello</t>
   </si>
   <si>
@@ -226,6 +220,21 @@
   </si>
   <si>
     <t>Spring Boot</t>
+  </si>
+  <si>
+    <t>Testes unitários das principais regras de negócio</t>
+  </si>
+  <si>
+    <t>Browser (Chrome, Firefox e Safari)</t>
+  </si>
+  <si>
+    <t>Azure (Aplicativos Web e Banco de Dados)</t>
+  </si>
+  <si>
+    <t>Autenticação de usuário</t>
+  </si>
+  <si>
+    <t>Logs de response (erros de servidor e da API)</t>
   </si>
 </sst>
 </file>
@@ -485,6 +494,78 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -494,9 +575,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -506,42 +584,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,39 +592,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -882,7 +891,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -895,33 +904,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40"/>
-      <c r="B1" s="41" t="s">
+      <c r="A1" s="31"/>
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="35"/>
       <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
@@ -933,19 +942,19 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="27" t="s">
+      <c r="A4" s="35"/>
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>53</v>
+      <c r="D4" s="22" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
@@ -957,19 +966,19 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="27" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="35"/>
       <c r="B7" s="5" t="s">
         <v>38</v>
       </c>
@@ -977,23 +986,23 @@
         <v>39</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="27" t="s">
+      <c r="A8" s="35"/>
+      <c r="B8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1005,46 +1014,46 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="27" t="s">
+      <c r="A10" s="35"/>
+      <c r="B10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>53</v>
+      <c r="D11" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1056,106 +1065,106 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="20" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>58</v>
+      <c r="D16" s="10" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="16"/>
-      <c r="B17" s="22" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>59</v>
+      <c r="D17" s="18" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="34" t="s">
-        <v>65</v>
+      <c r="D19" s="25" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>61</v>
+      <c r="D20" s="10" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="35" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="37" t="s">
-        <v>60</v>
+      <c r="D21" s="28" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>62</v>
+      <c r="D22" s="10" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="35" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="36" t="s">
+      <c r="C23" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="37" t="s">
-        <v>63</v>
+      <c r="D23" s="28" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="5" t="s">
         <v>18</v>
       </c>
@@ -1163,19 +1172,19 @@
         <v>31</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="31"/>
-      <c r="B25" s="38" t="s">
+      <c r="A25" s="42"/>
+      <c r="B25" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="39" t="s">
-        <v>53</v>
+      <c r="D25" s="30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>